<commit_message>
Finally was able to get single parameter sensitivity analysis to work.
</commit_message>
<xml_diff>
--- a/chrome-dithionite-tests/sensitivity/parameters.xlsx
+++ b/chrome-dithionite-tests/sensitivity/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="105" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="243" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -610,7 +610,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -638,16 +638,14 @@
         <v>5</v>
       </c>
       <c r="B2" s="0" t="n">
-        <f aca="false">LOG10(summary!B2)</f>
-        <v>-4.44249279809434</v>
+        <v>-5</v>
       </c>
       <c r="C2" s="0" t="n">
         <f aca="false">LOG10(summary!D2)</f>
         <v>-7</v>
       </c>
       <c r="D2" s="0" t="n">
-        <f aca="false">LOG10(summary!E2)</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,8 +678,7 @@
         <v>-7</v>
       </c>
       <c r="D4" s="0" t="n">
-        <f aca="false">LOG10(summary!E4)</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
minor. THIS IS THE SINGLE PARAM SENSITIVTY ANALYSIS BASE CASE
</commit_message>
<xml_diff>
--- a/chrome-dithionite-tests/sensitivity/parameters.xlsx
+++ b/chrome-dithionite-tests/sensitivity/parameters.xlsx
@@ -264,7 +264,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -610,7 +610,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -638,7 +638,8 @@
         <v>5</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>-5</v>
+        <f aca="false">LOG10(summary!B2)</f>
+        <v>-4.44249279809434</v>
       </c>
       <c r="C2" s="0" t="n">
         <f aca="false">LOG10(summary!D2)</f>

</xml_diff>

<commit_message>
Cleaned up code for single parameter sensitivity analysis and finalized.
</commit_message>
<xml_diff>
--- a/chrome-dithionite-tests/sensitivity/parameters.xlsx
+++ b/chrome-dithionite-tests/sensitivity/parameters.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="243" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="243" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="mads" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="mads_tightened" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>base</t>
   </si>
@@ -54,21 +55,33 @@
     <t>these are kept separate in the code, min and max should be multiplied by 175 for the paper</t>
   </si>
   <si>
+    <t>fraction</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>k_fe2_o2_fast</t>
+  </si>
+  <si>
+    <t>g mol^-1 s^-1</t>
+  </si>
+  <si>
+    <t>factor_k_fe2_o2_slow</t>
+  </si>
+  <si>
     <t>k_fe2_o2_slow</t>
   </si>
   <si>
-    <t>g mol^-1 s^-1</t>
-  </si>
-  <si>
-    <t>k_fe2_o2_fast</t>
+    <t>k_fe2_cr6_fast</t>
+  </si>
+  <si>
+    <t>factor_k_fe2_cr6_slow</t>
   </si>
   <si>
     <t>k_fe2_cr6_slow</t>
   </si>
   <si>
-    <t>k_fe2_cr6_fast</t>
-  </si>
-  <si>
     <t>is2o4</t>
   </si>
   <si>
@@ -145,6 +158,9 @@
   </si>
   <si>
     <t>ifeoh3</t>
+  </si>
+  <si>
+    <t>**cannot have fraction &gt; 1</t>
   </si>
 </sst>
 </file>
@@ -155,7 +171,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -180,6 +196,29 @@
     <font>
       <i val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF420E"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -227,7 +266,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,12 +275,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -253,6 +308,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -261,15 +376,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3979591836735"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6632653061224"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
@@ -293,57 +408,57 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>3.61E-005</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="4" t="n">
         <v>1E-007</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="4" t="n">
         <v>0.01</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="4" t="n">
         <v>0.001</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="4" t="n">
         <v>100</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <f aca="false">0.00001</f>
         <v>1E-005</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="4" t="n">
         <f aca="false">0.0000001</f>
         <v>1E-007</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="4" t="n">
         <f aca="false">0.01</f>
         <v>0.01</v>
       </c>
@@ -352,229 +467,265 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="4" t="n">
         <v>10000</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">1/1000</f>
+        <v>0.001</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <f aca="false">1/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <f aca="false">B7*B6</f>
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">B6*D7</f>
+        <v>0.01</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <f aca="false">B6*E7</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="D9" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E9" s="4" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D10" s="0" t="n">
+        <f aca="false">1/1000</f>
         <v>0.001</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2" t="n">
+      <c r="E10" s="0" t="n">
+        <f aca="false">1/10</f>
         <v>0.1</v>
       </c>
-      <c r="E8" s="2" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="0" t="n">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <f aca="false">B10*B9</f>
         <v>0.1</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="0" t="n">
+      <c r="D11" s="0" t="n">
+        <f aca="false">B9*D10</f>
         <v>0.01</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E11" s="0" t="n">
+        <f aca="false">B9*E10</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E12" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="n">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1" t="n">
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="n">
         <f aca="false">0.5/100</f>
         <v>0.005</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E13" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <f aca="false">B10/100*$B$18*($B$19/100^3)/($B$20/1000)</f>
+      <c r="F13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <f aca="false">B13/100*$B$21*($B$22/100^3)/($B$23/1000)</f>
         <v>0.00385814541031159</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">D10/100*$B$18*($B$19/100^3)/($B$20/1000)</f>
-        <v>1.9290727051558E-005</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <f aca="false">E10/100*$B$18*($B$19/100^3)/($B$20/1000)</f>
-        <v>0.019290727051558</v>
-      </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>1E-009</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>1E-012</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>1E-007</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <f aca="false">B13*$B$23</f>
-        <v>0.15</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="0" t="n">
-        <f aca="false">D13*$B$23</f>
+        <f aca="false">D13/100*$B$21*($B$22/100^3)/($B$23/1000)</f>
+        <v>1.9290727051558E-005</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">E13/100*$B$21*($B$22/100^3)/($B$23/1000)</f>
+        <v>0.019290727051558</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>1E-009</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>1E-012</v>
+      </c>
+      <c r="E15" s="4" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <f aca="false">B16*$B$26</f>
+        <v>0.15</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <f aca="false">D16*$B$26</f>
         <v>0.0015</v>
       </c>
-      <c r="E14" s="3" t="n">
+      <c r="E17" s="6" t="n">
         <v>15</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>1200</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>34.36</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="0" t="n">
-        <v>106.87</v>
-      </c>
-      <c r="C20" s="0" t="s">
+      <c r="B21" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -582,12 +733,34 @@
       <c r="A22" s="0" t="s">
         <v>37</v>
       </c>
+      <c r="B22" s="0" t="n">
+        <v>34.36</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" s="0" t="n">
+        <v>106.87</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="0" t="n">
         <v>0.15</v>
       </c>
     </row>
@@ -607,24 +780,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6632653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3214285714286"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
@@ -634,8 +807,9 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>5</v>
+      <c r="A2" s="0" t="str">
+        <f aca="false">summary!A2</f>
+        <v>k_s2o4_disp</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">LOG10(summary!B2)</f>
@@ -650,8 +824,9 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>7</v>
+      <c r="A3" s="0" t="str">
+        <f aca="false">summary!A3</f>
+        <v>k_s2o4_o2</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">LOG10(summary!B3)</f>
@@ -667,8 +842,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>41</v>
+      <c r="A4" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">LOG10(summary!B4)</f>
@@ -683,25 +858,27 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>12</v>
+      <c r="A5" s="0" t="str">
+        <f aca="false">summary!A5</f>
+        <v>fraction</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">LOG10(summary!B5)</f>
-        <v>-1</v>
+        <v>-0.301029995663981</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">LOG10(summary!D5)</f>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="D5" s="0" t="n">
-        <f aca="false">LOG10(summary!E5)</f>
-        <v>2</v>
+        <f aca="false">LOG10(summary!E6)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>14</v>
+      <c r="A6" s="0" t="str">
+        <f aca="false">summary!A6</f>
+        <v>k_fe2_o2_fast</v>
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">LOG10(summary!B6)</f>
@@ -717,105 +894,382 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>15</v>
+      <c r="A7" s="0" t="str">
+        <f aca="false">summary!A7</f>
+        <v>factor_k_fe2_o2_slow</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">LOG10(summary!B7)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">LOG10(summary!D7)</f>
         <v>-3</v>
       </c>
       <c r="D7" s="0" t="n">
-        <f aca="false">LOG10(summary!E7)</f>
-        <v>2</v>
+        <f aca="false">LOG10(summary!E9)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>16</v>
+      <c r="A8" s="0" t="str">
+        <f aca="false">summary!A9</f>
+        <v>k_fe2_cr6_fast</v>
       </c>
       <c r="B8" s="0" t="n">
-        <f aca="false">LOG10(summary!B8)</f>
+        <f aca="false">LOG10(summary!B9)</f>
         <v>1</v>
       </c>
       <c r="C8" s="0" t="n">
-        <f aca="false">LOG10(summary!D8)</f>
+        <f aca="false">LOG10(summary!D9)</f>
         <v>-1</v>
       </c>
       <c r="D8" s="0" t="n">
-        <f aca="false">LOG10(summary!E8)</f>
+        <f aca="false">LOG10(summary!E9)</f>
         <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>17</v>
+      <c r="A9" s="0" t="str">
+        <f aca="false">summary!A10</f>
+        <v>factor_k_fe2_cr6_slow</v>
       </c>
       <c r="B9" s="0" t="n">
-        <f aca="false">LOG10(summary!B9)</f>
-        <v>-1</v>
+        <f aca="false">LOG10(summary!B10)</f>
+        <v>-2</v>
       </c>
       <c r="C9" s="0" t="n">
-        <f aca="false">LOG10(summary!D9)</f>
-        <v>-2</v>
+        <f aca="false">LOG10(summary!D10)</f>
+        <v>-3</v>
       </c>
       <c r="D9" s="0" t="n">
-        <f aca="false">LOG10(summary!E9)</f>
-        <v>-0.301029995663981</v>
+        <f aca="false">LOG10(summary!D10)</f>
+        <v>-3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="n">
-        <f aca="false">LOG10(summary!B11)</f>
-        <v>-2.41362140818361</v>
+        <f aca="false">LOG10(summary!B12)</f>
+        <v>-1</v>
       </c>
       <c r="C10" s="0" t="n">
-        <f aca="false">LOG10(summary!D11)</f>
-        <v>-4.7146514038476</v>
+        <f aca="false">LOG10(summary!D12)</f>
+        <v>-2</v>
       </c>
       <c r="D10" s="0" t="n">
-        <f aca="false">LOG10(summary!E11)</f>
-        <v>-1.71465140384759</v>
+        <f aca="false">LOG10(summary!E12)</f>
+        <v>-0.301029995663981</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B11" s="0" t="n">
-        <f aca="false">LOG10(summary!B12)</f>
-        <v>-9</v>
+        <f aca="false">LOG10(summary!B14)</f>
+        <v>-2.41362140818361</v>
       </c>
       <c r="C11" s="0" t="n">
-        <f aca="false">LOG10(summary!D12)</f>
-        <v>-12</v>
+        <f aca="false">LOG10(summary!D14)</f>
+        <v>-4.7146514038476</v>
       </c>
       <c r="D11" s="0" t="n">
-        <f aca="false">LOG10(summary!E12)</f>
-        <v>-7</v>
+        <f aca="false">LOG10(summary!E14)</f>
+        <v>-1.7146514038476</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="n">
+        <f aca="false">LOG10(summary!B15)</f>
+        <v>-9</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <f aca="false">LOG10(summary!D15)</f>
+        <v>-12</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">LOG10(summary!E15)</f>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">LOG10(summary!B17)</f>
+        <v>-0.823908740944319</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <f aca="false">LOG10(summary!D17)</f>
+        <v>-2.82390874094432</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">LOG10(summary!E17)</f>
+        <v>1.17609125905568</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="str">
+        <f aca="false">mads!A2</f>
+        <v>k_s2o4_disp</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">LOG10(summary!B2)</f>
+        <v>-4.44249279809434</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <f aca="false">B2-1</f>
+        <v>-5.44249279809434</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">B2+1</f>
+        <v>-3.44249279809434</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="str">
+        <f aca="false">mads!A3</f>
+        <v>k_s2o4_o2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">LOG10(summary!B3)</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <f aca="false">B3-1</f>
+        <v>-1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">B3+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="str">
+        <f aca="false">mads!A4</f>
+        <v>k_s2o4_fe3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">LOG10(summary!B4)</f>
+        <v>-5</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">B4-1</f>
+        <v>-6</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">B4+1</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="str">
+        <f aca="false">mads!A5</f>
+        <v>fraction</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">LOG10(summary!B5)</f>
+        <v>-0.301029995663981</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">B5-1</f>
+        <v>-1.30102999566398</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <f aca="false">LOG10(1)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="str">
+        <f aca="false">mads!A6</f>
+        <v>k_fe2_o2_fast</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <f aca="false">LOG10(summary!B6)</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <f aca="false">B6-1</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">B6+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="str">
+        <f aca="false">mads!A7</f>
+        <v>factor_k_fe2_o2_slow</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <f aca="false">LOG10(summary!B7)</f>
+        <v>-2</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <f aca="false">B7-1</f>
+        <v>-3</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">B7+1</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="str">
+        <f aca="false">mads!A8</f>
+        <v>k_fe2_cr6_fast</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <f aca="false">LOG10(summary!B9)</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <f aca="false">B8-1</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">B8+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="str">
+        <f aca="false">mads!A9</f>
+        <v>factor_k_fe2_cr6_slow</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <f aca="false">LOG10(summary!B10)</f>
+        <v>-2</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <f aca="false">B9-1</f>
+        <v>-3</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">B9+1</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">LOG10(summary!B12)</f>
+        <v>-1</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <f aca="false">B10-1</f>
+        <v>-2</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">B10+1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="0" t="n">
         <f aca="false">LOG10(summary!B14)</f>
+        <v>-2.41362140818361</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <f aca="false">B11-1</f>
+        <v>-3.41362140818361</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">B11+1</f>
+        <v>-1.41362140818361</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">LOG10(summary!B15)</f>
+        <v>-9</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <f aca="false">B12-1</f>
+        <v>-10</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">B12+1</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">LOG10(summary!B17)</f>
         <v>-0.823908740944319</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <f aca="false">LOG10(summary!D14)</f>
-        <v>-2.82390874094432</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <f aca="false">LOG10(summary!E14)</f>
-        <v>1.17609125905568</v>
+      <c r="C13" s="0" t="n">
+        <f aca="false">B13-1</f>
+        <v>-1.82390874094432</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">B13+1</f>
+        <v>0.176091259055681</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started setting up mads files for full sensitivity analysis.
</commit_message>
<xml_diff>
--- a/chrome-dithionite-tests/sensitivity/parameters.xlsx
+++ b/chrome-dithionite-tests/sensitivity/parameters.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="243" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="243" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="mads" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="mads_tightened" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="mads_efast" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -378,7 +379,7 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1281,4 +1282,248 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="str">
+        <f aca="false">mads_tightened!A1</f>
+        <v>parameter</v>
+      </c>
+      <c r="B1" s="0" t="str">
+        <f aca="false">mads_tightened!B1</f>
+        <v>init</v>
+      </c>
+      <c r="C1" s="0" t="str">
+        <f aca="false">mads_tightened!C1</f>
+        <v>min</v>
+      </c>
+      <c r="D1" s="0" t="str">
+        <f aca="false">mads_tightened!D1</f>
+        <v>max</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="str">
+        <f aca="false">mads_tightened!A2</f>
+        <v>k_s2o4_disp</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">mads_tightened!B2</f>
+        <v>-4.44249279809434</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <f aca="false">mads_tightened!C2</f>
+        <v>-5.44249279809434</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">mads_tightened!D2</f>
+        <v>-3.44249279809434</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="str">
+        <f aca="false">mads_tightened!A3</f>
+        <v>k_s2o4_o2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">mads_tightened!B3</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <f aca="false">mads_tightened!C3</f>
+        <v>-1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">mads_tightened!D3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="str">
+        <f aca="false">mads_tightened!A4</f>
+        <v>k_s2o4_fe3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">mads_tightened!B4</f>
+        <v>-5</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">mads_tightened!C4</f>
+        <v>-6</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">mads_tightened!D4</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="str">
+        <f aca="false">mads_tightened!A5</f>
+        <v>fraction</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">mads_tightened!B5</f>
+        <v>-0.301029995663981</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">mads_tightened!C5</f>
+        <v>-1.30102999566398</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">mads_tightened!D5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="str">
+        <f aca="false">mads_tightened!A6</f>
+        <v>k_fe2_o2_fast</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <f aca="false">mads_tightened!B6</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <f aca="false">mads_tightened!C6</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">mads_tightened!D6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="str">
+        <f aca="false">mads_tightened!A7</f>
+        <v>factor_k_fe2_o2_slow</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <f aca="false">mads_tightened!B7</f>
+        <v>-2</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <f aca="false">mads_tightened!C7</f>
+        <v>-3</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">mads_tightened!D7</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="str">
+        <f aca="false">mads_tightened!A8</f>
+        <v>k_fe2_cr6_fast</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <f aca="false">mads_tightened!B8</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <f aca="false">mads_tightened!C8</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">mads_tightened!D8</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="str">
+        <f aca="false">mads_tightened!A9</f>
+        <v>factor_k_fe2_cr6_slow</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <f aca="false">mads_tightened!B9</f>
+        <v>-2</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <f aca="false">mads_tightened!C9</f>
+        <v>-3</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">mads_tightened!D9</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="str">
+        <f aca="false">mads_tightened!A10</f>
+        <v>is2o4</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">mads_tightened!B10</f>
+        <v>-1</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <f aca="false">mads_tightened!C10</f>
+        <v>-2</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">mads_tightened!D10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="str">
+        <f aca="false">mads_tightened!A11</f>
+        <v>ifeoh3</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">mads_tightened!B11</f>
+        <v>-2.41362140818361</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <f aca="false">mads_tightened!C11</f>
+        <v>-3.41362140818361</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">mads_tightened!D11</f>
+        <v>-1.41362140818361</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="str">
+        <f aca="false">mads_tightened!A13</f>
+        <v>q</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">mads_tightened!B13</f>
+        <v>-0.823908740944319</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <f aca="false">mads_tightened!C13</f>
+        <v>-1.82390874094432</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">mads_tightened!D13</f>
+        <v>0.176091259055681</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Preliminary full sensitivity analysis. Calibrate, LocalSA works. Calibraterandom, efast fail.
</commit_message>
<xml_diff>
--- a/chrome-dithionite-tests/sensitivity/parameters.xlsx
+++ b/chrome-dithionite-tests/sensitivity/parameters.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="243" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="419" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="mads" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="mads_tightened" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="mads_efast" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="mads_efast_tightened" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -172,7 +173,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -224,6 +225,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -267,7 +275,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -297,6 +305,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -380,7 +392,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1035,7 +1047,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1291,8 +1303,8 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1526,4 +1538,248 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="str">
+        <f aca="false">mads_efast!A1</f>
+        <v>parameter</v>
+      </c>
+      <c r="B1" s="0" t="str">
+        <f aca="false">mads_efast!B1</f>
+        <v>init</v>
+      </c>
+      <c r="C1" s="0" t="str">
+        <f aca="false">mads_efast!C1</f>
+        <v>min</v>
+      </c>
+      <c r="D1" s="0" t="str">
+        <f aca="false">mads_efast!D1</f>
+        <v>max</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="str">
+        <f aca="false">mads_efast!A2</f>
+        <v>k_s2o4_disp</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">mads_efast!B2</f>
+        <v>-4.44249279809434</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <f aca="false">B2-0.5</f>
+        <v>-4.94249279809434</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">B2+0.5</f>
+        <v>-3.94249279809434</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="str">
+        <f aca="false">mads_efast!A3</f>
+        <v>k_s2o4_o2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">mads_efast!B3</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <f aca="false">B3-0.5</f>
+        <v>-0.5</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">B3+0.5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="str">
+        <f aca="false">mads_efast!A4</f>
+        <v>k_s2o4_fe3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">mads_efast!B4</f>
+        <v>-5</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">B4-0.5</f>
+        <v>-5.5</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">B4+0.5</f>
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="str">
+        <f aca="false">mads_efast!A5</f>
+        <v>fraction</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">mads_efast!B5</f>
+        <v>-0.301029995663981</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">mads_efast!C5</f>
+        <v>-1.30102999566398</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <f aca="false">mads_efast!D5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="str">
+        <f aca="false">mads_efast!A6</f>
+        <v>k_fe2_o2_fast</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <f aca="false">mads_efast!B6</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <f aca="false">B6-0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">B6+0.5</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="str">
+        <f aca="false">mads_efast!A7</f>
+        <v>factor_k_fe2_o2_slow</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <f aca="false">mads_efast!B7</f>
+        <v>-2</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <f aca="false">B7-0.5</f>
+        <v>-2.5</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">B7+0.5</f>
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="str">
+        <f aca="false">mads_efast!A8</f>
+        <v>k_fe2_cr6_fast</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <f aca="false">mads_efast!B8</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <f aca="false">B8-0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">B8+0.5</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="str">
+        <f aca="false">mads_efast!A9</f>
+        <v>factor_k_fe2_cr6_slow</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <f aca="false">mads_efast!B9</f>
+        <v>-2</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <f aca="false">B9-0.5</f>
+        <v>-2.5</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">B9+0.5</f>
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="str">
+        <f aca="false">mads_efast!A10</f>
+        <v>is2o4</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">mads_efast!B10</f>
+        <v>-1</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <f aca="false">B10-0.5</f>
+        <v>-1.5</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">B10+0.5</f>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="str">
+        <f aca="false">mads_efast!A11</f>
+        <v>ifeoh3</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">mads_efast!B11</f>
+        <v>-2.41362140818361</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <f aca="false">B11-0.5</f>
+        <v>-2.91362140818361</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">B11+0.5</f>
+        <v>-1.91362140818361</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="str">
+        <f aca="false">mads_efast!A12</f>
+        <v>q</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">mads_efast!B12</f>
+        <v>-0.823908740944319</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <f aca="false">B12-0.5</f>
+        <v>-1.32390874094432</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">B12+0.5</f>
+        <v>-0.323908740944319</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Continue redoing mads sensitivity analysis.
</commit_message>
<xml_diff>
--- a/chrome-dithionite-tests/sensitivity/parameters.xlsx
+++ b/chrome-dithionite-tests/sensitivity/parameters.xlsx
@@ -5,21 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="209" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="883" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="mads" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="mads_tightened" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="mads_efast" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="mads_efast_tightened" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="mads_orig" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="mads" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="mads_tightened" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>base</t>
   </si>
@@ -103,12 +102,6 @@
   </si>
   <si>
     <t>M^3/m^3_bulk</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>m/s^2</t>
   </si>
   <si>
     <t>v</t>
@@ -177,7 +170,7 @@
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -223,6 +216,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FFFF420E"/>
       <name val="Arial"/>
@@ -231,7 +231,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFF3333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -279,7 +286,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -312,11 +319,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -333,7 +348,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -397,10 +412,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="1" sqref="C5:D5 D14"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -492,7 +507,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>13</v>
@@ -661,127 +676,109 @@
         <v>26</v>
       </c>
       <c r="B14" s="2" t="n">
-        <f aca="false">B13/100*$B$21*($B$22/100^3)/($B$23/1000)</f>
+        <f aca="false">B13/100*$B$19*($B$20/100^3)/($B$21/1000)</f>
         <v>0.00385814541031159</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="0" t="n">
-        <f aca="false">D13/100*$B$21*($B$22/100^3)/($B$23/1000)</f>
+        <f aca="false">D13/100*$B$19*($B$20/100^3)/($B$21/1000)</f>
         <v>1.9290727051558E-005</v>
       </c>
       <c r="E14" s="0" t="n">
-        <f aca="false">E13/100*$B$21*($B$22/100^3)/($B$23/1000)</f>
+        <f aca="false">E13/100*$B$19*($B$20/100^3)/($B$21/1000)</f>
         <v>0.019290727051558</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="3" t="n">
-        <v>1E-009</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="4" t="n">
-        <v>1E-012</v>
-      </c>
-      <c r="E15" s="4" t="n">
-        <v>1E-007</v>
-      </c>
-      <c r="F15" s="1"/>
+      <c r="D15" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="1" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="B16" s="2" t="n">
+        <f aca="false">B15*$B$24</f>
+        <v>0.15</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">D15*$B$24</f>
+        <v>0.0015</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="2" t="n">
-        <f aca="false">B16*$B$26</f>
-        <v>0.15</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <f aca="false">D16*$B$26</f>
-        <v>0.0015</v>
-      </c>
-      <c r="E17" s="6" t="n">
-        <v>15</v>
+      <c r="B19" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>34.36</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>1200</v>
+        <v>106.87</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>34.36</v>
-      </c>
-      <c r="C22" s="0" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="0" t="n">
-        <v>106.87</v>
-      </c>
-      <c r="C23" s="0" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="0" t="n">
+      <c r="B24" s="0" t="n">
         <v>0.15</v>
       </c>
     </row>
@@ -801,10 +798,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="1" sqref="C5:D5 C29"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -815,10 +812,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
@@ -863,8 +860,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>45</v>
+      <c r="A4" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">LOG10(summary!B4)</f>
@@ -885,7 +882,7 @@
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">LOG10(summary!B5)</f>
-        <v>-0.301029995663981</v>
+        <v>-0.221848749616356</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">LOG10(summary!D5)</f>
@@ -987,7 +984,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">LOG10(summary!B14)</f>
@@ -1004,35 +1001,18 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B12" s="0" t="n">
-        <f aca="false">LOG10(summary!B15)</f>
-        <v>-9</v>
+        <f aca="false">LOG10(summary!B16)</f>
+        <v>-0.823908740944319</v>
       </c>
       <c r="C12" s="0" t="n">
-        <f aca="false">LOG10(summary!D15)</f>
-        <v>-12</v>
+        <f aca="false">LOG10(summary!D16)</f>
+        <v>-2.82390874094432</v>
       </c>
       <c r="D12" s="0" t="n">
-        <f aca="false">LOG10(summary!E15)</f>
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <f aca="false">LOG10(summary!B17)</f>
-        <v>-0.823908740944319</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <f aca="false">LOG10(summary!D17)</f>
-        <v>-2.82390874094432</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <f aca="false">LOG10(summary!E17)</f>
+        <f aca="false">LOG10(summary!E16)</f>
         <v>1.17609125905568</v>
       </c>
     </row>
@@ -1052,10 +1032,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="1" sqref="C5:D5 D25"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1066,10 +1046,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
@@ -1080,7 +1060,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
-        <f aca="false">mads!A2</f>
+        <f aca="false">mads_orig!A2</f>
         <v>k_s2o4_disp</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -1098,7 +1078,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
-        <f aca="false">mads!A3</f>
+        <f aca="false">mads_orig!A3</f>
         <v>k_s2o4_o2</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -1116,7 +1096,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
-        <f aca="false">mads!A4</f>
+        <f aca="false">mads_orig!A4</f>
         <v>k_s2o4_fe3</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1134,28 +1114,28 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="str">
-        <f aca="false">mads!A5</f>
+        <f aca="false">mads_orig!A5</f>
         <v>fraction</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">LOG10(summary!B5)</f>
-        <v>-0.301029995663981</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <f aca="false">B5-1</f>
-        <v>-1.30102999566398</v>
-      </c>
-      <c r="D5" s="7" t="n">
+        <v>-0.221848749616356</v>
+      </c>
+      <c r="C5" s="9" t="n">
+        <f aca="false">LOG10(summary!D5)</f>
+        <v>-4</v>
+      </c>
+      <c r="D5" s="8" t="n">
         <f aca="false">LOG10(1)</f>
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="str">
-        <f aca="false">mads!A6</f>
+        <f aca="false">mads_orig!A6</f>
         <v>k_fe2_o2_fast</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -1172,8 +1152,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="str">
-        <f aca="false">mads!A7</f>
+      <c r="A7" s="8" t="str">
+        <f aca="false">mads_orig!A7</f>
         <v>factor_k_fe2_o2_slow</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -1191,7 +1171,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="str">
-        <f aca="false">mads!A8</f>
+        <f aca="false">mads_orig!A8</f>
         <v>k_fe2_cr6_fast</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -1208,8 +1188,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="str">
-        <f aca="false">mads!A9</f>
+      <c r="A9" s="8" t="str">
+        <f aca="false">mads_orig!A9</f>
         <v>factor_k_fe2_cr6_slow</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -1244,7 +1224,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">LOG10(summary!B14)</f>
@@ -1261,35 +1241,18 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B12" s="0" t="n">
-        <f aca="false">LOG10(summary!B15)</f>
-        <v>-9</v>
+        <f aca="false">LOG10(summary!B16)</f>
+        <v>-0.823908740944319</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">B12-1</f>
-        <v>-10</v>
+        <v>-1.82390874094432</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">B12+1</f>
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <f aca="false">LOG10(summary!B17)</f>
-        <v>-0.823908740944319</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <f aca="false">B13-1</f>
-        <v>-1.82390874094432</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <f aca="false">B13+1</f>
         <v>0.176091259055681</v>
       </c>
     </row>
@@ -1309,254 +1272,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="C5:D5 C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="str">
-        <f aca="false">mads_tightened!A1</f>
-        <v>parameter</v>
-      </c>
-      <c r="B1" s="0" t="str">
-        <f aca="false">mads_tightened!B1</f>
-        <v>init</v>
-      </c>
-      <c r="C1" s="0" t="str">
-        <f aca="false">mads_tightened!C1</f>
-        <v>min</v>
-      </c>
-      <c r="D1" s="0" t="str">
-        <f aca="false">mads_tightened!D1</f>
-        <v>max</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="str">
-        <f aca="false">mads_tightened!A2</f>
-        <v>k_s2o4_disp</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <f aca="false">mads_tightened!B2</f>
-        <v>-4.44249279809434</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <f aca="false">mads_tightened!C2</f>
-        <v>-5.44249279809434</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">mads_tightened!D2</f>
-        <v>-3.44249279809434</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="str">
-        <f aca="false">mads_tightened!A3</f>
-        <v>k_s2o4_o2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <f aca="false">mads_tightened!B3</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <f aca="false">mads_tightened!C3</f>
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">mads_tightened!D3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="str">
-        <f aca="false">mads_tightened!A4</f>
-        <v>k_s2o4_fe3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <f aca="false">mads_tightened!B4</f>
-        <v>-5</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <f aca="false">mads_tightened!C4</f>
-        <v>-6</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">mads_tightened!D4</f>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="str">
-        <f aca="false">mads_tightened!A5</f>
-        <v>fraction</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <f aca="false">mads_tightened!B5</f>
-        <v>-0.301029995663981</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <f aca="false">mads_tightened!C5</f>
-        <v>-1.30102999566398</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">mads_tightened!D5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="str">
-        <f aca="false">mads_tightened!A6</f>
-        <v>k_fe2_o2_fast</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <f aca="false">mads_tightened!B6</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <f aca="false">mads_tightened!C6</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <f aca="false">mads_tightened!D6</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="str">
-        <f aca="false">mads_tightened!A7</f>
-        <v>factor_k_fe2_o2_slow</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <f aca="false">mads_tightened!B7</f>
-        <v>-2</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <f aca="false">mads_tightened!C7</f>
-        <v>-3</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <f aca="false">mads_tightened!D7</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="str">
-        <f aca="false">mads_tightened!A8</f>
-        <v>k_fe2_cr6_fast</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <f aca="false">mads_tightened!B8</f>
-        <v>1</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <f aca="false">mads_tightened!C8</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <f aca="false">mads_tightened!D8</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="str">
-        <f aca="false">mads_tightened!A9</f>
-        <v>factor_k_fe2_cr6_slow</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <f aca="false">mads_tightened!B9</f>
-        <v>-2</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <f aca="false">mads_tightened!C9</f>
-        <v>-3</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <f aca="false">mads_tightened!D9</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="str">
-        <f aca="false">mads_tightened!A10</f>
-        <v>is2o4</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <f aca="false">mads_tightened!B10</f>
-        <v>-1</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <f aca="false">mads_tightened!C10</f>
-        <v>-2</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <f aca="false">mads_tightened!D10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="str">
-        <f aca="false">mads_tightened!A11</f>
-        <v>ifeoh3</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <f aca="false">mads_tightened!B11</f>
-        <v>-2.41362140818361</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <f aca="false">mads_tightened!C11</f>
-        <v>-3.41362140818361</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">mads_tightened!D11</f>
-        <v>-1.41362140818361</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="str">
-        <f aca="false">mads_tightened!A13</f>
-        <v>q</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <f aca="false">mads_tightened!B13</f>
-        <v>-0.823908740944319</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <f aca="false">mads_tightened!C13</f>
-        <v>-1.82390874094432</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <f aca="false">mads_tightened!D13</f>
-        <v>0.176091259055681</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="C5:D5 B11"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1566,239 +1285,221 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="str">
-        <f aca="false">mads_efast!A1</f>
-        <v>parameter</v>
-      </c>
-      <c r="B1" s="0" t="str">
-        <f aca="false">mads_efast!B1</f>
-        <v>init</v>
-      </c>
-      <c r="C1" s="0" t="str">
-        <f aca="false">mads_efast!C1</f>
-        <v>min</v>
-      </c>
-      <c r="D1" s="0" t="str">
-        <f aca="false">mads_efast!D1</f>
-        <v>max</v>
+      <c r="A1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
-        <f aca="false">mads_efast!A2</f>
+        <f aca="false">mads_orig!A2</f>
         <v>k_s2o4_disp</v>
       </c>
       <c r="B2" s="0" t="n">
-        <f aca="false">mads_efast!B2</f>
+        <f aca="false">mads_orig!B2</f>
         <v>-4.44249279809434</v>
       </c>
-      <c r="C2" s="8" t="n">
-        <f aca="false">B2-F3</f>
+      <c r="C2" s="10" t="n">
+        <f aca="false">B2-F2</f>
         <v>-4.54249279809434</v>
       </c>
-      <c r="D2" s="8" t="n">
-        <f aca="false">B2+F3</f>
+      <c r="D2" s="10" t="n">
+        <f aca="false">B2+F2</f>
         <v>-4.34249279809434</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>48</v>
+      <c r="F2" s="7" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
-        <f aca="false">mads_efast!A3</f>
+        <f aca="false">mads_orig!A3</f>
         <v>k_s2o4_o2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <f aca="false">mads_efast!B3</f>
+        <f aca="false">mads_orig!B3</f>
         <v>0</v>
       </c>
       <c r="C3" s="0" t="n">
-        <f aca="false">B3-F3</f>
+        <f aca="false">B3-F2</f>
         <v>-0.1</v>
       </c>
       <c r="D3" s="0" t="n">
-        <f aca="false">B3+F3</f>
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="0" t="n">
+        <f aca="false">B3+F2</f>
         <v>0.1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
-        <f aca="false">mads_efast!A4</f>
+        <f aca="false">mads_orig!A4</f>
         <v>k_s2o4_fe3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <f aca="false">mads_efast!B4</f>
+        <f aca="false">mads_orig!B4</f>
         <v>-5</v>
       </c>
       <c r="C4" s="0" t="n">
-        <f aca="false">B4-F3</f>
+        <f aca="false">B4-F2</f>
         <v>-5.1</v>
       </c>
       <c r="D4" s="0" t="n">
-        <f aca="false">B4+F3</f>
+        <f aca="false">B4+F2</f>
         <v>-4.9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="str">
-        <f aca="false">mads_efast!A5</f>
+        <f aca="false">mads_orig!A5</f>
         <v>fraction</v>
       </c>
       <c r="B5" s="0" t="n">
-        <f aca="false">mads_efast!B5</f>
-        <v>-0.301029995663981</v>
-      </c>
-      <c r="C5" s="8" t="n">
-        <f aca="false">B5-0.1</f>
-        <v>-0.401029995663981</v>
-      </c>
-      <c r="D5" s="9" t="n">
-        <f aca="false">B5+0.1</f>
-        <v>-0.201029995663981</v>
+        <f aca="false">mads_orig!B5</f>
+        <v>-0.221848749616356</v>
+      </c>
+      <c r="C5" s="10" t="n">
+        <f aca="false">B5-F2</f>
+        <v>-0.321848749616356</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <f aca="false">B5+F2</f>
+        <v>-0.121848749616356</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="str">
-        <f aca="false">mads_efast!A6</f>
+        <f aca="false">mads_orig!A6</f>
         <v>k_fe2_o2_fast</v>
       </c>
       <c r="B6" s="0" t="n">
-        <f aca="false">mads_efast!B6</f>
+        <f aca="false">mads_orig!B6</f>
         <v>1</v>
       </c>
       <c r="C6" s="0" t="n">
-        <f aca="false">B6-F3</f>
+        <f aca="false">B6-F2</f>
         <v>0.9</v>
       </c>
       <c r="D6" s="0" t="n">
-        <f aca="false">B6+F3</f>
+        <f aca="false">B6+F2</f>
         <v>1.1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="str">
-        <f aca="false">mads_efast!A7</f>
+        <f aca="false">mads_orig!A7</f>
         <v>factor_k_fe2_o2_slow</v>
       </c>
       <c r="B7" s="0" t="n">
-        <f aca="false">mads_efast!B7</f>
+        <f aca="false">mads_orig!B7</f>
         <v>-2</v>
       </c>
       <c r="C7" s="0" t="n">
-        <f aca="false">B7-F3</f>
+        <f aca="false">B7-F2</f>
         <v>-2.1</v>
       </c>
       <c r="D7" s="0" t="n">
-        <f aca="false">B7+F3</f>
+        <f aca="false">B7+F2</f>
         <v>-1.9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="str">
-        <f aca="false">mads_efast!A8</f>
+        <f aca="false">mads_orig!A8</f>
         <v>k_fe2_cr6_fast</v>
       </c>
       <c r="B8" s="0" t="n">
-        <f aca="false">mads_efast!B8</f>
+        <f aca="false">mads_orig!B8</f>
         <v>1</v>
       </c>
       <c r="C8" s="0" t="n">
-        <f aca="false">B8-F3</f>
+        <f aca="false">B8-F2</f>
         <v>0.9</v>
       </c>
       <c r="D8" s="0" t="n">
-        <f aca="false">B8+F3</f>
+        <f aca="false">B8+F2</f>
         <v>1.1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="str">
-        <f aca="false">mads_efast!A9</f>
+        <f aca="false">mads_orig!A9</f>
         <v>factor_k_fe2_cr6_slow</v>
       </c>
       <c r="B9" s="0" t="n">
-        <f aca="false">mads_efast!B9</f>
+        <f aca="false">mads_orig!B9</f>
         <v>-2</v>
       </c>
       <c r="C9" s="0" t="n">
-        <f aca="false">B9-F3</f>
+        <f aca="false">B9-F2</f>
         <v>-2.1</v>
       </c>
       <c r="D9" s="0" t="n">
-        <f aca="false">B9+F3</f>
+        <f aca="false">B9+F2</f>
         <v>-1.9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="str">
-        <f aca="false">mads_efast!A10</f>
+        <f aca="false">mads_orig!A10</f>
         <v>is2o4</v>
       </c>
       <c r="B10" s="0" t="n">
-        <f aca="false">mads_efast!B10</f>
+        <f aca="false">mads_orig!B10</f>
         <v>-1</v>
       </c>
       <c r="C10" s="0" t="n">
-        <f aca="false">B10-F3</f>
+        <f aca="false">B10-F2</f>
         <v>-1.1</v>
       </c>
       <c r="D10" s="0" t="n">
-        <f aca="false">B10+F3</f>
+        <f aca="false">B10+F2</f>
         <v>-0.9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="str">
-        <f aca="false">mads_efast!A11</f>
+        <f aca="false">mads_orig!A11</f>
         <v>ifeoh3</v>
       </c>
       <c r="B11" s="0" t="n">
-        <f aca="false">mads_efast!B11</f>
+        <f aca="false">mads_orig!B11</f>
         <v>-2.41362140818361</v>
       </c>
-      <c r="C11" s="8" t="n">
-        <f aca="false">B11-F3</f>
+      <c r="C11" s="10" t="n">
+        <f aca="false">B11-F2</f>
         <v>-2.51362140818361</v>
       </c>
-      <c r="D11" s="8" t="n">
-        <f aca="false">B11+F3</f>
+      <c r="D11" s="10" t="n">
+        <f aca="false">B11+F2</f>
         <v>-2.31362140818361</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="str">
-        <f aca="false">mads_efast!A12</f>
+        <f aca="false">mads_orig!A12</f>
         <v>q</v>
       </c>
       <c r="B12" s="0" t="n">
-        <f aca="false">mads_efast!B12</f>
+        <f aca="false">mads_orig!B12</f>
         <v>-0.823908740944319</v>
       </c>
-      <c r="C12" s="8" t="n">
-        <f aca="false">B12-F3</f>
+      <c r="C12" s="10" t="n">
+        <f aca="false">B12-F2</f>
         <v>-0.923908740944319</v>
       </c>
-      <c r="D12" s="8" t="n">
-        <f aca="false">B12+F3</f>
+      <c r="D12" s="10" t="n">
+        <f aca="false">B12+F2</f>
         <v>-0.723908740944319</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="n">
-        <f aca="false">10^B5</f>
-        <v>0.5</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <f aca="false">10^C5</f>
-        <v>0.397164117362141</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <f aca="false">10^D5</f>
-        <v>0.629462705897084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to figure out what is wrong with pflotran-dithionite-new.
</commit_message>
<xml_diff>
--- a/chrome-dithionite-tests/sensitivity/parameters.xlsx
+++ b/chrome-dithionite-tests/sensitivity/parameters.xlsx
@@ -5,20 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="883" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="884" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="mads_orig" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="mads" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="mads_tightened" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="mads" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="mads_tightened" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>base</t>
   </si>
@@ -150,9 +149,6 @@
   </si>
   <si>
     <t>k_s2o4_fe3</t>
-  </si>
-  <si>
-    <t>ifeoh3</t>
   </si>
   <si>
     <t>**cannot have fraction &gt; 1</t>
@@ -170,7 +166,7 @@
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -224,21 +220,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF420E"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF3333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFF420E"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -331,7 +320,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,7 +337,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -415,7 +404,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -448,7 +437,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>3.61E-005</v>
+        <v>3.16227766016838E-005</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>
@@ -507,7 +496,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>13</v>
@@ -798,10 +787,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -831,14 +820,15 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">LOG10(summary!B2)</f>
-        <v>-4.44249279809434</v>
+        <v>-4.5</v>
       </c>
       <c r="C2" s="0" t="n">
-        <f aca="false">LOG10(summary!D2)</f>
-        <v>-7</v>
+        <f aca="false">B2-1</f>
+        <v>-5.5</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>-3</v>
+        <f aca="false">B2+1</f>
+        <v>-3.5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,12 +841,12 @@
         <v>0</v>
       </c>
       <c r="C3" s="0" t="n">
-        <f aca="false">LOG10(summary!D3)</f>
-        <v>-3</v>
+        <f aca="false">B3-1</f>
+        <v>-1</v>
       </c>
       <c r="D3" s="0" t="n">
-        <f aca="false">LOG10(summary!E3)</f>
-        <v>2</v>
+        <f aca="false">B3+1</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -868,29 +858,33 @@
         <v>-5</v>
       </c>
       <c r="C4" s="0" t="n">
-        <f aca="false">LOG10(summary!D4)</f>
-        <v>-7</v>
+        <f aca="false">B4-1</f>
+        <v>-6</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>-3</v>
+        <f aca="false">B4+1</f>
+        <v>-4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="str">
-        <f aca="false">summary!A5</f>
+        <f aca="false">['file:///mnt/madskil_scratch/Programs/pflotran-dithionite-new/dithionite_sensitivity/parameters.xlsx']summary!A5</f>
         <v>fraction</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">LOG10(summary!B5)</f>
-        <v>-0.221848749616356</v>
+        <v>-0.301029995663981</v>
       </c>
       <c r="C5" s="0" t="n">
-        <f aca="false">LOG10(summary!D5)</f>
-        <v>-4</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">LOG10(summary!E6)</f>
-        <v>4</v>
+        <f aca="false">B5-1</f>
+        <v>-1.30102999566398</v>
+      </c>
+      <c r="D5" s="9" t="n">
+        <f aca="false">LOG10(1)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,17 +897,17 @@
         <v>1</v>
       </c>
       <c r="C6" s="0" t="n">
-        <f aca="false">LOG10(summary!D6)</f>
-        <v>-1</v>
+        <f aca="false">B6-1</f>
+        <v>0</v>
       </c>
       <c r="D6" s="0" t="n">
-        <f aca="false">LOG10(summary!E6)</f>
-        <v>4</v>
+        <f aca="false">B6+1</f>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="str">
-        <f aca="false">summary!A7</f>
+        <f aca="false">['file:///mnt/madskil_scratch/Programs/pflotran-dithionite-new/dithionite_sensitivity/parameters.xlsx']summary!A7</f>
         <v>factor_k_fe2_o2_slow</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -921,17 +915,17 @@
         <v>-2</v>
       </c>
       <c r="C7" s="0" t="n">
-        <f aca="false">LOG10(summary!D7)</f>
+        <f aca="false">B7-1</f>
         <v>-3</v>
       </c>
       <c r="D7" s="0" t="n">
-        <f aca="false">LOG10(summary!E9)</f>
-        <v>4</v>
+        <f aca="false">B7+1</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="str">
-        <f aca="false">summary!A9</f>
+        <f aca="false">['file:///mnt/madskil_scratch/Programs/pflotran-dithionite-new/dithionite_sensitivity/parameters.xlsx']summary!A9</f>
         <v>k_fe2_cr6_fast</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -939,17 +933,17 @@
         <v>1</v>
       </c>
       <c r="C8" s="0" t="n">
-        <f aca="false">LOG10(summary!D9)</f>
-        <v>-1</v>
+        <f aca="false">B8-1</f>
+        <v>0</v>
       </c>
       <c r="D8" s="0" t="n">
-        <f aca="false">LOG10(summary!E9)</f>
-        <v>4</v>
+        <f aca="false">B8+1</f>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="str">
-        <f aca="false">summary!A10</f>
+        <f aca="false">['file:///mnt/madskil_scratch/Programs/pflotran-dithionite-new/dithionite_sensitivity/parameters.xlsx']summary!A10</f>
         <v>factor_k_fe2_cr6_slow</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -957,63 +951,66 @@
         <v>-2</v>
       </c>
       <c r="C9" s="0" t="n">
-        <f aca="false">LOG10(summary!D10)</f>
+        <f aca="false">B9-1</f>
         <v>-3</v>
       </c>
       <c r="D9" s="0" t="n">
-        <f aca="false">LOG10(summary!D10)</f>
-        <v>-3</v>
+        <f aca="false">B9+1</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>21</v>
+      <c r="A10" s="0" t="str">
+        <f aca="false">summary!A12</f>
+        <v>is2o4</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">LOG10(summary!B12)</f>
         <v>-1</v>
       </c>
       <c r="C10" s="0" t="n">
-        <f aca="false">LOG10(summary!D12)</f>
+        <f aca="false">B10-1</f>
         <v>-2</v>
       </c>
       <c r="D10" s="0" t="n">
-        <f aca="false">LOG10(summary!E12)</f>
-        <v>-0.301029995663981</v>
+        <f aca="false">B10+1</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>44</v>
+      <c r="A11" s="0" t="str">
+        <f aca="false">summary!A14</f>
+        <v>ifeoh3_vf</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">LOG10(summary!B14)</f>
         <v>-2.41362140818361</v>
       </c>
       <c r="C11" s="0" t="n">
-        <f aca="false">LOG10(summary!D14)</f>
-        <v>-4.7146514038476</v>
+        <f aca="false">B11-1</f>
+        <v>-3.41362140818361</v>
       </c>
       <c r="D11" s="0" t="n">
-        <f aca="false">LOG10(summary!E14)</f>
-        <v>-1.7146514038476</v>
+        <f aca="false">B11+1</f>
+        <v>-1.41362140818361</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>31</v>
+      <c r="A12" s="0" t="str">
+        <f aca="false">summary!A16</f>
+        <v>q</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">LOG10(summary!B16)</f>
         <v>-0.823908740944319</v>
       </c>
       <c r="C12" s="0" t="n">
-        <f aca="false">LOG10(summary!D16)</f>
-        <v>-2.82390874094432</v>
+        <f aca="false">B12-1</f>
+        <v>-1.82390874094432</v>
       </c>
       <c r="D12" s="0" t="n">
-        <f aca="false">LOG10(summary!E16)</f>
-        <v>1.17609125905568</v>
+        <f aca="false">B12+1</f>
+        <v>0.176091259055681</v>
       </c>
     </row>
   </sheetData>
@@ -1032,250 +1029,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="str">
-        <f aca="false">mads_orig!A2</f>
-        <v>k_s2o4_disp</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <f aca="false">LOG10(summary!B2)</f>
-        <v>-4.44249279809434</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <f aca="false">B2-1</f>
-        <v>-5.44249279809434</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">B2+1</f>
-        <v>-3.44249279809434</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="str">
-        <f aca="false">mads_orig!A3</f>
-        <v>k_s2o4_o2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <f aca="false">LOG10(summary!B3)</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <f aca="false">B3-1</f>
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">B3+1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="str">
-        <f aca="false">mads_orig!A4</f>
-        <v>k_s2o4_fe3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <f aca="false">LOG10(summary!B4)</f>
-        <v>-5</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <f aca="false">B4-1</f>
-        <v>-6</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">B4+1</f>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="str">
-        <f aca="false">mads_orig!A5</f>
-        <v>fraction</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <f aca="false">LOG10(summary!B5)</f>
-        <v>-0.221848749616356</v>
-      </c>
-      <c r="C5" s="9" t="n">
-        <f aca="false">LOG10(summary!D5)</f>
-        <v>-4</v>
-      </c>
-      <c r="D5" s="8" t="n">
-        <f aca="false">LOG10(1)</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="str">
-        <f aca="false">mads_orig!A6</f>
-        <v>k_fe2_o2_fast</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <f aca="false">LOG10(summary!B6)</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <f aca="false">B6-1</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <f aca="false">B6+1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="str">
-        <f aca="false">mads_orig!A7</f>
-        <v>factor_k_fe2_o2_slow</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <f aca="false">LOG10(summary!B7)</f>
-        <v>-2</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <f aca="false">B7-1</f>
-        <v>-3</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <f aca="false">B7+1</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="str">
-        <f aca="false">mads_orig!A8</f>
-        <v>k_fe2_cr6_fast</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <f aca="false">LOG10(summary!B9)</f>
-        <v>1</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <f aca="false">B8-1</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <f aca="false">B8+1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="str">
-        <f aca="false">mads_orig!A9</f>
-        <v>factor_k_fe2_cr6_slow</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <f aca="false">LOG10(summary!B10)</f>
-        <v>-2</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <f aca="false">B9-1</f>
-        <v>-3</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <f aca="false">B9+1</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <f aca="false">LOG10(summary!B12)</f>
-        <v>-1</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <f aca="false">B10-1</f>
-        <v>-2</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <f aca="false">B10+1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <f aca="false">LOG10(summary!B14)</f>
-        <v>-2.41362140818361</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <f aca="false">B11-1</f>
-        <v>-3.41362140818361</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">B11+1</f>
-        <v>-1.41362140818361</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <f aca="false">LOG10(summary!B16)</f>
-        <v>-0.823908740944319</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <f aca="false">B12-1</f>
-        <v>-1.82390874094432</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <f aca="false">B12+1</f>
-        <v>0.176091259055681</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1298,25 +1055,25 @@
         <v>3</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
-        <f aca="false">mads_orig!A2</f>
+        <f aca="false">mads!A2</f>
         <v>k_s2o4_disp</v>
       </c>
       <c r="B2" s="0" t="n">
-        <f aca="false">mads_orig!B2</f>
-        <v>-4.44249279809434</v>
+        <f aca="false">LOG10(summary!B2)</f>
+        <v>-4.5</v>
       </c>
       <c r="C2" s="10" t="n">
         <f aca="false">B2-F2</f>
-        <v>-4.54249279809434</v>
+        <v>-4.6</v>
       </c>
       <c r="D2" s="10" t="n">
         <f aca="false">B2+F2</f>
-        <v>-4.34249279809434</v>
+        <v>-4.4</v>
       </c>
       <c r="F2" s="7" t="n">
         <v>0.1</v>
@@ -1324,11 +1081,11 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
-        <f aca="false">mads_orig!A3</f>
+        <f aca="false">mads!A3</f>
         <v>k_s2o4_o2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <f aca="false">mads_orig!B3</f>
+        <f aca="false">LOG10(summary!B3)</f>
         <v>0</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -1342,11 +1099,11 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
-        <f aca="false">mads_orig!A4</f>
+        <f aca="false">mads!A4</f>
         <v>k_s2o4_fe3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <f aca="false">mads_orig!B4</f>
+        <f aca="false">LOG10(summary!B4)</f>
         <v>-5</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -1360,29 +1117,29 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="str">
-        <f aca="false">mads_orig!A5</f>
+        <f aca="false">mads!A5</f>
         <v>fraction</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <f aca="false">mads_orig!B5</f>
-        <v>-0.221848749616356</v>
+      <c r="B5" s="8" t="n">
+        <f aca="false">LOG10(summary!B5)</f>
+        <v>-0.301029995663981</v>
       </c>
       <c r="C5" s="10" t="n">
         <f aca="false">B5-F2</f>
-        <v>-0.321848749616356</v>
+        <v>-0.401029995663981</v>
       </c>
       <c r="D5" s="11" t="n">
         <f aca="false">B5+F2</f>
-        <v>-0.121848749616356</v>
+        <v>-0.201029995663981</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="str">
-        <f aca="false">mads_orig!A6</f>
+        <f aca="false">mads!A6</f>
         <v>k_fe2_o2_fast</v>
       </c>
       <c r="B6" s="0" t="n">
-        <f aca="false">mads_orig!B6</f>
+        <f aca="false">LOG10(summary!B6)</f>
         <v>1</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -1396,11 +1153,11 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="str">
-        <f aca="false">mads_orig!A7</f>
+        <f aca="false">mads!A7</f>
         <v>factor_k_fe2_o2_slow</v>
       </c>
       <c r="B7" s="0" t="n">
-        <f aca="false">mads_orig!B7</f>
+        <f aca="false">LOG10(summary!B7)</f>
         <v>-2</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -1414,11 +1171,11 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="str">
-        <f aca="false">mads_orig!A8</f>
+        <f aca="false">mads!A8</f>
         <v>k_fe2_cr6_fast</v>
       </c>
       <c r="B8" s="0" t="n">
-        <f aca="false">mads_orig!B8</f>
+        <f aca="false">LOG10(summary!B9)</f>
         <v>1</v>
       </c>
       <c r="C8" s="0" t="n">
@@ -1432,11 +1189,11 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="str">
-        <f aca="false">mads_orig!A9</f>
+        <f aca="false">mads!A9</f>
         <v>factor_k_fe2_cr6_slow</v>
       </c>
       <c r="B9" s="0" t="n">
-        <f aca="false">mads_orig!B9</f>
+        <f aca="false">LOG10(summary!B10)</f>
         <v>-2</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -1450,11 +1207,11 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="str">
-        <f aca="false">mads_orig!A10</f>
+        <f aca="false">mads!A10</f>
         <v>is2o4</v>
       </c>
       <c r="B10" s="0" t="n">
-        <f aca="false">mads_orig!B10</f>
+        <f aca="false">LOG10(summary!B12)</f>
         <v>-1</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -1468,11 +1225,11 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="str">
-        <f aca="false">mads_orig!A11</f>
-        <v>ifeoh3</v>
+        <f aca="false">mads!A11</f>
+        <v>ifeoh3_vf</v>
       </c>
       <c r="B11" s="0" t="n">
-        <f aca="false">mads_orig!B11</f>
+        <f aca="false">LOG10(summary!B14)</f>
         <v>-2.41362140818361</v>
       </c>
       <c r="C11" s="10" t="n">
@@ -1486,11 +1243,11 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="str">
-        <f aca="false">mads_orig!A12</f>
+        <f aca="false">mads!A12</f>
         <v>q</v>
       </c>
       <c r="B12" s="0" t="n">
-        <f aca="false">mads_orig!B12</f>
+        <f aca="false">LOG10(summary!B16)</f>
         <v>-0.823908740944319</v>
       </c>
       <c r="C12" s="10" t="n">

</xml_diff>